<commit_message>
Normalizacion aplicativo contenedor carpetas
</commit_message>
<xml_diff>
--- a/Dia 9 (Buscador de Objetos)/pythonProject/Liquidacion/formatos/formato_liquidacion_consolidada_detallado.xlsx
+++ b/Dia 9 (Buscador de Objetos)/pythonProject/Liquidacion/formatos/formato_liquidacion_consolidada_detallado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgiraldo\Documents\git\Course_Python_Total\Dia 9 (Buscador de Objetos)\pythonProject\Liquidacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgiraldo\Documents\git\Course_Python_Total\Dia 9 (Buscador de Objetos)\pythonProject\Liquidacion\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E502B354-7216-45C8-AB9F-26757B0684E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2969DA-59A5-4F8A-B04A-7F4B88E02B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fondo Usos" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>Fondo General  Usos 2200</t>
-  </si>
-  <si>
     <t>Fondo General  Usos 2400</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>Fondo General  Usos 2700</t>
+  </si>
+  <si>
+    <t>Fondo General  Usos 2900</t>
   </si>
 </sst>
 </file>
@@ -643,18 +643,45 @@
     <xf numFmtId="173" fontId="4" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="2" borderId="12" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="2" borderId="15" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="2" borderId="13" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="12" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="15" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="13" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -664,38 +691,11 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="2" borderId="12" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="2" borderId="15" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="2" borderId="13" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="12" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="15" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="13" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -812,14 +812,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -891,14 +891,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -970,14 +970,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1294,8 +1294,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1315,65 +1315,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="56"/>
+      <c r="E1" s="52"/>
       <c r="F1" s="4"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="3"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
       <c r="F3" s="3"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="3"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="2:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43" t="str">
+      <c r="B5" s="54" t="str">
         <f ca="1">"Fecha de Proceso: "&amp;TEXT(TODAY(),"dd/mm/yyyy")</f>
-        <v>Fecha de Proceso: 02/02/2024</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+        <v>Fecha de Proceso: 23/02/2024</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
     </row>
     <row r="6" spans="2:9" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="45" t="s">
+      <c r="E6" s="45"/>
+      <c r="F6" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="45"/>
+      <c r="H6" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="46"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="47"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="27" t="s">
         <v>11</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="C17" s="37"/>
       <c r="D17" s="31"/>
       <c r="E17" s="40"/>
-      <c r="F17" s="60"/>
+      <c r="F17" s="43"/>
       <c r="G17" s="41"/>
       <c r="H17" s="38"/>
       <c r="I17" s="39"/>
@@ -1589,7 +1589,7 @@
     <row r="24" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6"/>
       <c r="C24" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="34">
         <f t="shared" ref="D24:I24" si="0">SUM(D8:D23)</f>
@@ -1619,51 +1619,51 @@
     <row r="25" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
       <c r="C25" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="50">
+        <v>14</v>
+      </c>
+      <c r="D25" s="46">
         <f>D24+F24+H24</f>
         <v>0</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53">
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49">
         <f>E24+G24+I24</f>
         <v>0</v>
       </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="55"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="51"/>
     </row>
     <row r="26" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="D1:E4"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1699,47 +1699,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="58"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="4"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="3"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
       <c r="F3" s="3"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="3"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="2:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43" t="str">
+      <c r="B5" s="54" t="str">
         <f ca="1">'Fondo Usos'!B5:C5</f>
-        <v>Fecha de Proceso: 02/02/2024</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+        <v>Fecha de Proceso: 23/02/2024</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
     </row>
     <row r="6" spans="2:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="57" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="59" t="s">
@@ -1748,8 +1748,8 @@
       <c r="E6" s="59"/>
     </row>
     <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="27" t="s">
         <v>7</v>
       </c>
@@ -1868,45 +1868,45 @@
         <f>SUM(E8:E22)</f>
         <v>442711140</v>
       </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="D1:E4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="D1:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -1941,47 +1941,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="58"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="4"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="3"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
       <c r="F3" s="3"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="3"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="2:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43" t="str">
+      <c r="B5" s="54" t="str">
         <f ca="1">'Fondo Usos'!B5:C5</f>
-        <v>Fecha de Proceso: 02/02/2024</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+        <v>Fecha de Proceso: 23/02/2024</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
     </row>
     <row r="6" spans="2:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="57" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="59" t="s">
@@ -1990,8 +1990,8 @@
       <c r="E6" s="59"/>
     </row>
     <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="27" t="s">
         <v>8</v>
       </c>
@@ -2111,45 +2111,45 @@
         <f>SUM(E8:E22)</f>
         <v>4304000</v>
       </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="D1:E4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="D1:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>